<commit_message>
Restructuring and formatting code
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohitvernekar/Projects/RAG-Retrieval-Comparision/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEC94F1-834F-3A49-AD4E-8411654C27D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D10D1F-63F3-8243-B2BE-09E185547FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="3800" windowWidth="28040" windowHeight="17440" xr2:uid="{53C0EC21-998D-934E-948C-9830CF4B554C}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{53C0EC21-998D-934E-948C-9830CF4B554C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Model</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Dot Product</t>
   </si>
   <si>
-    <t>Euclidean Dist.</t>
-  </si>
-  <si>
     <t>MiniLM (msmarco-MiniLM-L12-cos-v5)</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>BERT</t>
+  </si>
+  <si>
+    <t>MPNet (all-mpnet-base-v2)</t>
   </si>
 </sst>
 </file>
@@ -133,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -193,11 +193,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -205,12 +242,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -219,6 +250,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB79EC5-872E-1747-8E3E-2809DF05F0A2}">
-  <dimension ref="B2:H15"/>
+  <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="188" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B7"/>
+    <sheetView tabSelected="1" zoomScale="266" zoomScaleNormal="221" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,93 +663,93 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
-        <v>18</v>
+      <c r="B4" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="4">
-        <v>0.15166666666666601</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="E4" s="4">
-        <v>0.41033333333333299</v>
+        <v>0.5</v>
       </c>
       <c r="F4" s="4">
-        <v>0.37382996031746002</v>
+        <v>0.36833333333333301</v>
       </c>
       <c r="G4" s="4">
-        <v>0.38076865079365002</v>
+        <v>0.36833333333333301</v>
       </c>
       <c r="H4" s="4">
-        <v>0.51703972885300498</v>
+        <v>0.52368858663467499</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="5"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="4">
-        <v>0.15233333333333299</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="E5" s="4">
-        <v>0.40849999999999997</v>
+        <v>0.5</v>
       </c>
       <c r="F5" s="4">
-        <v>0.36860317460317399</v>
+        <v>0.37166666666666598</v>
       </c>
       <c r="G5" s="4">
-        <v>0.37616190476190398</v>
+        <v>0.37</v>
       </c>
       <c r="H5" s="4">
-        <v>0.51280867837455901</v>
+        <v>0.526191934123447</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="5"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4">
-        <v>0.14000000000000001</v>
+        <v>6.6666666666666596E-2</v>
       </c>
       <c r="E6" s="4">
-        <v>0.37366666666666598</v>
+        <v>0.2</v>
       </c>
       <c r="F6" s="4">
-        <v>0.34866329365079302</v>
+        <v>0.26095238095237999</v>
       </c>
       <c r="G6" s="4">
-        <v>0.36192420634920602</v>
+        <v>0.26095238095237999</v>
       </c>
       <c r="H6" s="4">
-        <v>0.49765236808039398</v>
+        <v>0.438698234078569</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="5"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" s="4">
-        <v>0.14799999999999999</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="E7" s="4">
-        <v>0.39500000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="F7" s="4">
-        <v>0.36765813492063398</v>
+        <v>0.353333333333333</v>
       </c>
       <c r="G7" s="4">
-        <v>0.37548412698412698</v>
+        <v>0.353333333333333</v>
       </c>
       <c r="H7" s="4">
-        <v>0.51189899866438304</v>
+        <v>0.46409951840956998</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -726,7 +772,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -747,7 +793,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -770,7 +816,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
@@ -814,17 +860,17 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>9</v>
@@ -847,7 +893,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>9</v>
@@ -868,14 +914,37 @@
         <v>0.69504294159075497</v>
       </c>
     </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.266666666666666</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0.67833333333333301</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.75537193629320898</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B13:H13"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B13:H13"/>
   </mergeCells>
-  <conditionalFormatting sqref="D14:D15 D3:D12">
+  <conditionalFormatting sqref="D14:D16 D3:D12">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -887,7 +956,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E15 E3:E12">
+  <conditionalFormatting sqref="E14:E16 E3:E12">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -899,7 +968,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F15 F3:F12">
+  <conditionalFormatting sqref="F14:F16 F3:F12">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -911,7 +980,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14:G15 G3:G12">
+  <conditionalFormatting sqref="G14:G16 G3:G12">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -923,7 +992,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:H15 H3:H12">
+  <conditionalFormatting sqref="H14:H16 H3:H12">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>